<commit_message>
more testing on more systems
</commit_message>
<xml_diff>
--- a/rasppi-3b_results.xlsx
+++ b/rasppi-3b_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\astei\Documents\dev\memory_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{501D656D-E534-4FAB-8D3A-A78F8B31152D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0317F18E-E31B-4CDD-B39C-3F5A7167480B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20715" yWindow="-18015" windowWidth="27120" windowHeight="19110"/>
+    <workbookView xWindow="12195" yWindow="-12015" windowWidth="8850" windowHeight="6240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'res2'!$A$1:$K$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'res2'!$A$1:$K$361</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -2065,7 +2065,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2593,11 +2593,11 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2613,11 +2613,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2930,12 +2930,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -15564,9 +15564,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K142"/>
+  <autoFilter ref="A1:K361" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="B1:D1048576">
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="int64_t">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="int64_t">
       <formula>NOT(ISERROR(SEARCH("int64_t",B1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="double">
@@ -15584,7 +15584,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>